<commit_message>
Reading production units coords from Excel
</commit_message>
<xml_diff>
--- a/server/test/data/production_units.xlsx
+++ b/server/test/data/production_units.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>nome</t>
   </si>
@@ -107,15 +107,28 @@
   </si>
   <si>
     <t>BM-BAR-1</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -130,7 +143,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -138,13 +151,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,22 +512,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="22.25" customWidth="1"/>
     <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="5" max="5" width="17.125" customWidth="1"/>
+    <col min="5" max="5" width="21.625" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
     <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="15" max="15" width="13.75" customWidth="1"/>
+    <col min="16" max="16" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -539,8 +572,14 @@
       <c r="N1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -556,8 +595,14 @@
       <c r="N2">
         <v>302000.3</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" s="2">
+        <v>-21.23799528</v>
+      </c>
+      <c r="P2" s="2">
+        <v>-39.962888059999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -567,8 +612,14 @@
       <c r="D3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3" s="2">
+        <v>-21.338045829999999</v>
+      </c>
+      <c r="P3" s="2">
+        <v>-40.057548330000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -578,8 +629,14 @@
       <c r="D4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4" s="2">
+        <v>-25.54349861</v>
+      </c>
+      <c r="P4" s="2">
+        <v>-42.841819170000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -589,8 +646,14 @@
       <c r="D5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5" s="2">
+        <v>-25.672804169999999</v>
+      </c>
+      <c r="P5" s="2">
+        <v>-43.206191939999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -603,8 +666,14 @@
       <c r="E6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6" s="2">
+        <v>-25.14156917</v>
+      </c>
+      <c r="P6" s="2">
+        <v>-42.94469694</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -614,8 +683,14 @@
       <c r="D7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7" s="2">
+        <v>-26.466638329999999</v>
+      </c>
+      <c r="P7" s="2">
+        <v>-46.528688330000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -625,8 +700,14 @@
       <c r="D8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8" s="2">
+        <v>-25.204078330000002</v>
+      </c>
+      <c r="P8" s="2">
+        <v>-42.878562780000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -636,8 +717,14 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9" s="2">
+        <v>-25.448848609999999</v>
+      </c>
+      <c r="P9" s="2">
+        <v>-42.753071939999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -647,8 +734,15 @@
       <c r="D10" t="s">
         <v>15</v>
       </c>
+      <c r="O10" s="2">
+        <v>-22.496580000000002</v>
+      </c>
+      <c r="P10" s="2">
+        <v>-39.937440279999997</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>